<commit_message>
Updated Columns in DT Sheet
</commit_message>
<xml_diff>
--- a/timetabledatabase/CivilEngineering.xlsx
+++ b/timetabledatabase/CivilEngineering.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\timetabledatabase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01B2B2B-5E18-4548-A78D-A23758F67D03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{CF5458FB-8CE1-4942-AFB2-3465C6397638}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="FE" sheetId="1" r:id="rId1"/>
@@ -19,7 +18,7 @@
     <sheet name="BE" sheetId="4" r:id="rId4"/>
     <sheet name="DT" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
   <si>
     <t>Subject</t>
   </si>
@@ -42,11 +41,47 @@
   <si>
     <t>End-Time</t>
   </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>ExamTitle</t>
+  </si>
+  <si>
+    <t>NumSub</t>
+  </si>
+  <si>
+    <t>Shipbuild</t>
+  </si>
+  <si>
+    <t>Wednesday 21/07/2021</t>
+  </si>
+  <si>
+    <t>15:43</t>
+  </si>
+  <si>
+    <t>16:43</t>
+  </si>
+  <si>
+    <t>FE</t>
+  </si>
+  <si>
+    <t>Civil Engineering</t>
+  </si>
+  <si>
+    <t>INTERN TEST</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -391,22 +426,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4EA95A6-741C-448D-80AC-C48FC9448DD1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="A1:D1048576"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.5546875" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -426,22 +461,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB8F965C-2E44-4EC8-BB52-EDC5228C2D74}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.5546875" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -461,22 +496,93 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D7232F2-C250-4CF7-A999-AB5C1107DB8B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="false">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.5546875" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row spans="1:4" x14ac:dyDescent="0.3" outlineLevel="0" r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row spans="1:4" x14ac:dyDescent="0.3" outlineLevel="0" r="2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="3">
+      <c r="A3" s="0" t="inlineStr">
+        <is>
+          <t>adwbqqb</t>
+        </is>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>Tuesday 20/07/2021</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>15:57</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>15:57</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1048576"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.5546875" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -495,51 +601,71 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC17D91-76A8-400F-9C2F-B8340704DE5B}">
-  <dimension ref="A1:D1"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" customWidth="1"/>
+    <col min="3" max="3" width="29.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row spans="1:4" x14ac:dyDescent="0.3" outlineLevel="0" r="1">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row spans="1:4" x14ac:dyDescent="0.3" outlineLevel="0" r="2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="3">
+      <c r="A3" s="0" t="inlineStr">
+        <is>
+          <t>TE</t>
+        </is>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>Civil Engineering</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>qrbqwqtbqwbqtbb</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6693CEB7-969C-44F6-9D15-D1F16FAA1434}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>